<commit_message>
updates for new file of provide with cmd command
</commit_message>
<xml_diff>
--- a/provide/test/TestDataProvideSBS.xlsx
+++ b/provide/test/TestDataProvideSBS.xlsx
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF1" sqref="AF1:AG1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>